<commit_message>
added additionnal histograms that compare different configurations for the same diameter range
</commit_message>
<xml_diff>
--- a/excel/example.jpg.xlsx
+++ b/excel/example.jpg.xlsx
@@ -26,7 +26,7 @@
     <t>Chart categories</t>
   </si>
   <si>
-    <t>Number of droplets (example.jpg)</t>
+    <t>example.jpg</t>
   </si>
 </sst>
 </file>
@@ -109,58 +109,37 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Number of droplets (example.jpg)</c:v>
+                  <c:v>example.jpg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Plot!$B$2:$B$12</c:f>
+              <c:f>Plot!$B$2:$B$5</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0 - 0.35</c:v>
+                  <c:v>0 - 0.15 µm</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35 - 0.7</c:v>
+                  <c:v>0.15 - 0.6 µm</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7 - 1.05</c:v>
+                  <c:v>0.6 - 2 µm</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.05 - 1.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4 - 1.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.75 - 2.1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.1 - 2.45</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.45 - 2.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8 - 3.15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.15 - 3.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>&gt;3.5</c:v>
+                  <c:v>&gt;2 µm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plot!$C$2:$C$12</c:f>
+              <c:f>Plot!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -171,27 +150,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -288,10 +246,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -598,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,24 +575,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="B2" t="str">
-        <f>"0 - "&amp;'Plot'!A2&amp;""</f>
-        <v>0 - 0.35</v>
+        <f>"0 - "&amp;'Plot'!A2&amp;" µm"</f>
+        <v>0 - 0.15 µm</v>
       </c>
       <c r="C2">
-        <f t="array" ref="C2:C12">frequency('Droplet diameters'!A2:A12,'Plot'!A2:A11)</f>
+        <f t="array" ref="C2:C5">frequency('Droplet diameters'!A2:A12,'Plot'!A2:A4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="B3" t="str">
-        <f>""&amp;'Plot'!A2&amp;" - "&amp;'Plot'!A3&amp;""</f>
-        <v>0.35 - 0.7</v>
+        <f>""&amp;'Plot'!A2&amp;" - "&amp;'Plot'!A3&amp;" µm"</f>
+        <v>0.15 - 0.6 µm</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -642,106 +600,22 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1.05</v>
+        <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f>""&amp;'Plot'!A3&amp;" - "&amp;'Plot'!A4&amp;""</f>
-        <v>0.7 - 1.05</v>
+        <f>""&amp;'Plot'!A3&amp;" - "&amp;'Plot'!A4&amp;" µm"</f>
+        <v>0.6 - 2 µm</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5">
-        <v>1.4</v>
-      </c>
       <c r="B5" t="str">
-        <f>""&amp;'Plot'!A4&amp;" - "&amp;'Plot'!A5&amp;""</f>
-        <v>1.05 - 1.4</v>
+        <f>"&gt;"&amp;'Plot'!A4&amp;" µm"</f>
+        <v>&gt;2 µm</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>1.75</v>
-      </c>
-      <c r="B6" t="str">
-        <f>""&amp;'Plot'!A5&amp;" - "&amp;'Plot'!A6&amp;""</f>
-        <v>1.4 - 1.75</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>2.1</v>
-      </c>
-      <c r="B7" t="str">
-        <f>""&amp;'Plot'!A6&amp;" - "&amp;'Plot'!A7&amp;""</f>
-        <v>1.75 - 2.1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>2.45</v>
-      </c>
-      <c r="B8" t="str">
-        <f>""&amp;'Plot'!A7&amp;" - "&amp;'Plot'!A8&amp;""</f>
-        <v>2.1 - 2.45</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>2.8</v>
-      </c>
-      <c r="B9" t="str">
-        <f>""&amp;'Plot'!A8&amp;" - "&amp;'Plot'!A9&amp;""</f>
-        <v>2.45 - 2.8</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>3.15</v>
-      </c>
-      <c r="B10" t="str">
-        <f>""&amp;'Plot'!A9&amp;" - "&amp;'Plot'!A10&amp;""</f>
-        <v>2.8 - 3.15</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>3.5</v>
-      </c>
-      <c r="B11" t="str">
-        <f>""&amp;'Plot'!A10&amp;" - "&amp;'Plot'!A11&amp;""</f>
-        <v>3.15 - 3.5</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="str">
-        <f>"&gt;"&amp;'Plot'!A11&amp;""</f>
-        <v>&gt;3.5</v>
-      </c>
-      <c r="C12">
         <v>0</v>
       </c>
     </row>

</xml_diff>